<commit_message>
updates in the movement class
</commit_message>
<xml_diff>
--- a/matrix.xlsx
+++ b/matrix.xlsx
@@ -358,7 +358,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -390,13 +390,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <v>15</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added a user interface in the command prompt and a log file
</commit_message>
<xml_diff>
--- a/matrix.xlsx
+++ b/matrix.xlsx
@@ -71,9 +71,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -358,7 +357,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -378,25 +377,25 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
+      <c r="A2">
         <v>10</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B3">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C3">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -411,7 +410,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E9" s="2"/>
+      <c r="E9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>